<commit_message>
Codigo em python finalizado
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Sara</t>
-  </si>
-  <si>
     <t>nome</t>
   </si>
   <si>
     <t>telefone</t>
+  </si>
+  <si>
+    <t>Bbzinha</t>
   </si>
 </sst>
 </file>
@@ -69,7 +69,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -377,24 +377,21 @@
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="B2" s="2">
+        <v>558586441988</v>
       </c>
-      <c r="B2" s="2">
-        <v>5585994326521</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>